<commit_message>
SO Test Cases issues clean up
</commit_message>
<xml_diff>
--- a/templates/QARSF/CustomerMaster.xlsx
+++ b/templates/QARSF/CustomerMaster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\QARSF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\QARSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4809A3E8-EAA5-41B3-A618-DC6293721066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6781CEF1-B70F-4CD4-9F71-E3D36A651086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1020" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader_Invoicing&amp;Credit" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="30">
   <si>
     <t>API Mode</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>a5B41000000PRNX</t>
+  </si>
+  <si>
+    <t>AutomationCust-3</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -553,7 +556,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6737F574-F797-4D90-9E07-D5E83E892D4B}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31AFFEF-D881-4A16-95BC-C259D062DE49}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>

</xml_diff>